<commit_message>
working version of html tool with multiple files
</commit_message>
<xml_diff>
--- a/input/Thyristors_Diodes_Disks.xlsx
+++ b/input/Thyristors_Diodes_Disks.xlsx
@@ -1,15 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basov\Documents\_WORK IFX\SoftProjects\product_selection_guide_builder\input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$1</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -3424,8 +3432,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3501,6 +3509,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3547,7 +3563,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3579,9 +3595,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3613,6 +3630,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3788,14 +3806,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M351"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="18.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3836,7 +3859,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3877,7 +3900,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3918,7 +3941,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -3959,7 +3982,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -4000,7 +4023,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4041,7 +4064,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -4082,7 +4105,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -4123,7 +4146,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -4164,7 +4187,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -4205,7 +4228,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -4246,7 +4269,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -4287,7 +4310,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -4328,7 +4351,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -4369,7 +4392,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -4410,7 +4433,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -4451,7 +4474,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -4492,7 +4515,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -4533,7 +4556,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -4574,7 +4597,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -4615,7 +4638,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -4656,7 +4679,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -4697,7 +4720,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -4738,7 +4761,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -4779,7 +4802,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -4820,7 +4843,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -4861,7 +4884,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -4902,7 +4925,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -4943,7 +4966,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -4984,7 +5007,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -5025,7 +5048,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -5066,7 +5089,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -5107,7 +5130,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -5148,7 +5171,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -5189,7 +5212,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -5230,7 +5253,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -5271,7 +5294,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -5312,7 +5335,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -5353,7 +5376,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -5394,7 +5417,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -5435,7 +5458,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -5476,7 +5499,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -5517,7 +5540,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -5558,7 +5581,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -5599,7 +5622,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -5640,7 +5663,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -5681,7 +5704,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -5722,7 +5745,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -5763,7 +5786,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -5804,7 +5827,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -5845,7 +5868,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -5886,7 +5909,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -5927,7 +5950,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -5968,7 +5991,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -6009,7 +6032,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -6050,7 +6073,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -6091,7 +6114,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -6132,7 +6155,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -6173,7 +6196,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -6214,7 +6237,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>71</v>
       </c>
@@ -6255,7 +6278,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -6296,7 +6319,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>73</v>
       </c>
@@ -6337,7 +6360,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -6378,7 +6401,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -6419,7 +6442,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>76</v>
       </c>
@@ -6460,7 +6483,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -6501,7 +6524,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -6542,7 +6565,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -6583,7 +6606,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -6624,7 +6647,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -6665,7 +6688,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -6706,7 +6729,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -6747,7 +6770,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>84</v>
       </c>
@@ -6788,7 +6811,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -6829,7 +6852,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -6870,7 +6893,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -6911,7 +6934,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>88</v>
       </c>
@@ -6952,7 +6975,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>89</v>
       </c>
@@ -6993,7 +7016,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>90</v>
       </c>
@@ -7034,7 +7057,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -7075,7 +7098,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>92</v>
       </c>
@@ -7116,7 +7139,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>93</v>
       </c>
@@ -7157,7 +7180,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>94</v>
       </c>
@@ -7198,7 +7221,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>95</v>
       </c>
@@ -7239,7 +7262,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>96</v>
       </c>
@@ -7280,7 +7303,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>97</v>
       </c>
@@ -7321,7 +7344,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>98</v>
       </c>
@@ -7362,7 +7385,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>99</v>
       </c>
@@ -7403,7 +7426,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>100</v>
       </c>
@@ -7444,7 +7467,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>101</v>
       </c>
@@ -7485,7 +7508,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>102</v>
       </c>
@@ -7526,7 +7549,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>103</v>
       </c>
@@ -7567,7 +7590,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>104</v>
       </c>
@@ -7608,7 +7631,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>105</v>
       </c>
@@ -7649,7 +7672,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>106</v>
       </c>
@@ -7690,7 +7713,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>107</v>
       </c>
@@ -7731,7 +7754,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>108</v>
       </c>
@@ -7772,7 +7795,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>109</v>
       </c>
@@ -7813,7 +7836,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>110</v>
       </c>
@@ -7854,7 +7877,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>111</v>
       </c>
@@ -7895,7 +7918,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>112</v>
       </c>
@@ -7936,7 +7959,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>113</v>
       </c>
@@ -7977,7 +8000,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>114</v>
       </c>
@@ -8018,7 +8041,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>115</v>
       </c>
@@ -8059,7 +8082,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>116</v>
       </c>
@@ -8100,7 +8123,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>117</v>
       </c>
@@ -8141,7 +8164,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>118</v>
       </c>
@@ -8182,7 +8205,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>119</v>
       </c>
@@ -8223,7 +8246,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="109" spans="1:13">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>120</v>
       </c>
@@ -8264,7 +8287,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>121</v>
       </c>
@@ -8305,7 +8328,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="111" spans="1:13">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>122</v>
       </c>
@@ -8346,7 +8369,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>123</v>
       </c>
@@ -8387,7 +8410,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="113" spans="1:13">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>124</v>
       </c>
@@ -8428,7 +8451,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="114" spans="1:13">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>125</v>
       </c>
@@ -8469,7 +8492,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>126</v>
       </c>
@@ -8510,7 +8533,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="116" spans="1:13">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>127</v>
       </c>
@@ -8551,7 +8574,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="117" spans="1:13">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>128</v>
       </c>
@@ -8592,7 +8615,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="118" spans="1:13">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>129</v>
       </c>
@@ -8633,7 +8656,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>130</v>
       </c>
@@ -8674,7 +8697,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>131</v>
       </c>
@@ -8715,7 +8738,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>132</v>
       </c>
@@ -8756,7 +8779,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>133</v>
       </c>
@@ -8797,7 +8820,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>134</v>
       </c>
@@ -8838,7 +8861,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>135</v>
       </c>
@@ -8879,7 +8902,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>136</v>
       </c>
@@ -8920,7 +8943,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>137</v>
       </c>
@@ -8961,7 +8984,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>138</v>
       </c>
@@ -9002,7 +9025,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>139</v>
       </c>
@@ -9043,7 +9066,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>140</v>
       </c>
@@ -9084,7 +9107,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>141</v>
       </c>
@@ -9125,7 +9148,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="131" spans="1:13">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>142</v>
       </c>
@@ -9166,7 +9189,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="132" spans="1:13">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>143</v>
       </c>
@@ -9207,7 +9230,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="133" spans="1:13">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>144</v>
       </c>
@@ -9248,7 +9271,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="134" spans="1:13">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>145</v>
       </c>
@@ -9289,7 +9312,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>146</v>
       </c>
@@ -9330,7 +9353,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="136" spans="1:13">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>147</v>
       </c>
@@ -9371,7 +9394,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="137" spans="1:13">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>148</v>
       </c>
@@ -9412,7 +9435,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="138" spans="1:13">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>149</v>
       </c>
@@ -9453,7 +9476,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="139" spans="1:13">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>150</v>
       </c>
@@ -9494,7 +9517,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="140" spans="1:13">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>151</v>
       </c>
@@ -9535,7 +9558,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="141" spans="1:13">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>152</v>
       </c>
@@ -9576,7 +9599,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="142" spans="1:13">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>153</v>
       </c>
@@ -9617,7 +9640,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="143" spans="1:13">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>154</v>
       </c>
@@ -9658,7 +9681,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="144" spans="1:13">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>155</v>
       </c>
@@ -9699,7 +9722,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>156</v>
       </c>
@@ -9740,7 +9763,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="146" spans="1:13">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>157</v>
       </c>
@@ -9781,7 +9804,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>158</v>
       </c>
@@ -9822,7 +9845,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>159</v>
       </c>
@@ -9863,7 +9886,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="149" spans="1:13">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>160</v>
       </c>
@@ -9904,7 +9927,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>161</v>
       </c>
@@ -9945,7 +9968,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>162</v>
       </c>
@@ -9986,7 +10009,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>163</v>
       </c>
@@ -10027,7 +10050,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>164</v>
       </c>
@@ -10068,7 +10091,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>165</v>
       </c>
@@ -10109,7 +10132,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="155" spans="1:13">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>166</v>
       </c>
@@ -10150,7 +10173,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="156" spans="1:13">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>167</v>
       </c>
@@ -10191,7 +10214,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="157" spans="1:13">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>168</v>
       </c>
@@ -10232,7 +10255,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="158" spans="1:13">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>169</v>
       </c>
@@ -10273,7 +10296,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>170</v>
       </c>
@@ -10314,7 +10337,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>171</v>
       </c>
@@ -10355,7 +10378,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="161" spans="1:13">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>172</v>
       </c>
@@ -10396,7 +10419,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="162" spans="1:13">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>173</v>
       </c>
@@ -10437,7 +10460,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>174</v>
       </c>
@@ -10478,7 +10501,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="164" spans="1:13">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>175</v>
       </c>
@@ -10519,7 +10542,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>176</v>
       </c>
@@ -10560,7 +10583,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>177</v>
       </c>
@@ -10601,7 +10624,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="167" spans="1:13">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>178</v>
       </c>
@@ -10642,7 +10665,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>179</v>
       </c>
@@ -10683,7 +10706,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>180</v>
       </c>
@@ -10724,7 +10747,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="170" spans="1:13">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>181</v>
       </c>
@@ -10765,7 +10788,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>182</v>
       </c>
@@ -10806,7 +10829,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="172" spans="1:13">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>183</v>
       </c>
@@ -10847,7 +10870,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="173" spans="1:13">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>184</v>
       </c>
@@ -10888,7 +10911,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="174" spans="1:13">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>185</v>
       </c>
@@ -10929,7 +10952,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="175" spans="1:13">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>186</v>
       </c>
@@ -10970,7 +10993,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="176" spans="1:13">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>187</v>
       </c>
@@ -11011,7 +11034,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>188</v>
       </c>
@@ -11052,7 +11075,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="178" spans="1:13">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>189</v>
       </c>
@@ -11093,7 +11116,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="179" spans="1:13">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>190</v>
       </c>
@@ -11134,7 +11157,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>191</v>
       </c>
@@ -11175,7 +11198,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="181" spans="1:13">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>192</v>
       </c>
@@ -11216,7 +11239,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="182" spans="1:13">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>193</v>
       </c>
@@ -11257,7 +11280,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="183" spans="1:13">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>194</v>
       </c>
@@ -11298,7 +11321,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="184" spans="1:13">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>195</v>
       </c>
@@ -11339,7 +11362,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="185" spans="1:13">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>196</v>
       </c>
@@ -11380,7 +11403,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="186" spans="1:13">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>197</v>
       </c>
@@ -11421,7 +11444,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="187" spans="1:13">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>198</v>
       </c>
@@ -11462,7 +11485,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="188" spans="1:13">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>199</v>
       </c>
@@ -11503,7 +11526,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="189" spans="1:13">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>200</v>
       </c>
@@ -11544,7 +11567,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="190" spans="1:13">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>201</v>
       </c>
@@ -11585,7 +11608,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="191" spans="1:13">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>202</v>
       </c>
@@ -11626,7 +11649,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="192" spans="1:13">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>203</v>
       </c>
@@ -11667,7 +11690,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="193" spans="1:13">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>204</v>
       </c>
@@ -11708,7 +11731,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="194" spans="1:13">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>205</v>
       </c>
@@ -11749,7 +11772,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>206</v>
       </c>
@@ -11790,7 +11813,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>207</v>
       </c>
@@ -11831,7 +11854,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="197" spans="1:13">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>208</v>
       </c>
@@ -11872,7 +11895,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="198" spans="1:13">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>209</v>
       </c>
@@ -11913,7 +11936,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="199" spans="1:13">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>210</v>
       </c>
@@ -11954,7 +11977,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="200" spans="1:13">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>211</v>
       </c>
@@ -11995,7 +12018,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="201" spans="1:13">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>212</v>
       </c>
@@ -12036,7 +12059,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="202" spans="1:13">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>213</v>
       </c>
@@ -12077,7 +12100,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="203" spans="1:13">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>214</v>
       </c>
@@ -12118,7 +12141,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="204" spans="1:13">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>215</v>
       </c>
@@ -12159,7 +12182,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="205" spans="1:13">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>216</v>
       </c>
@@ -12200,7 +12223,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="206" spans="1:13">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>217</v>
       </c>
@@ -12241,7 +12264,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="207" spans="1:13">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>218</v>
       </c>
@@ -12282,7 +12305,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="208" spans="1:13">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>219</v>
       </c>
@@ -12323,7 +12346,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="209" spans="1:13">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>220</v>
       </c>
@@ -12364,7 +12387,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="210" spans="1:13">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>221</v>
       </c>
@@ -12405,7 +12428,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="211" spans="1:13">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>222</v>
       </c>
@@ -12446,7 +12469,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="212" spans="1:13">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>223</v>
       </c>
@@ -12487,7 +12510,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="213" spans="1:13">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>224</v>
       </c>
@@ -12528,7 +12551,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="214" spans="1:13">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>225</v>
       </c>
@@ -12569,7 +12592,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="215" spans="1:13">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>226</v>
       </c>
@@ -12610,7 +12633,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="216" spans="1:13">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>227</v>
       </c>
@@ -12651,7 +12674,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="217" spans="1:13">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>228</v>
       </c>
@@ -12692,7 +12715,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="218" spans="1:13">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>229</v>
       </c>
@@ -12733,7 +12756,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="219" spans="1:13">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>230</v>
       </c>
@@ -12774,7 +12797,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="220" spans="1:13">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>231</v>
       </c>
@@ -12815,7 +12838,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="221" spans="1:13">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>232</v>
       </c>
@@ -12856,7 +12879,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="222" spans="1:13">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>233</v>
       </c>
@@ -12897,7 +12920,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="223" spans="1:13">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>234</v>
       </c>
@@ -12938,7 +12961,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="224" spans="1:13">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>235</v>
       </c>
@@ -12979,7 +13002,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="225" spans="1:13">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>236</v>
       </c>
@@ -13020,7 +13043,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="226" spans="1:13">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>237</v>
       </c>
@@ -13061,7 +13084,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="227" spans="1:13">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>238</v>
       </c>
@@ -13102,7 +13125,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="228" spans="1:13">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>239</v>
       </c>
@@ -13143,7 +13166,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="229" spans="1:13">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>240</v>
       </c>
@@ -13184,7 +13207,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="230" spans="1:13">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>241</v>
       </c>
@@ -13225,7 +13248,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="231" spans="1:13">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>242</v>
       </c>
@@ -13266,7 +13289,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="232" spans="1:13">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>243</v>
       </c>
@@ -13307,7 +13330,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="233" spans="1:13">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>244</v>
       </c>
@@ -13348,7 +13371,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="234" spans="1:13">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>245</v>
       </c>
@@ -13389,7 +13412,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="235" spans="1:13">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>246</v>
       </c>
@@ -13430,7 +13453,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="236" spans="1:13">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>247</v>
       </c>
@@ -13471,7 +13494,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="237" spans="1:13">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>248</v>
       </c>
@@ -13512,7 +13535,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="238" spans="1:13">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>249</v>
       </c>
@@ -13553,7 +13576,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="239" spans="1:13">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>250</v>
       </c>
@@ -13594,7 +13617,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="240" spans="1:13">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>251</v>
       </c>
@@ -13635,7 +13658,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="241" spans="1:13">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>252</v>
       </c>
@@ -13676,7 +13699,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="242" spans="1:13">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>253</v>
       </c>
@@ -13717,7 +13740,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="243" spans="1:13">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>254</v>
       </c>
@@ -13758,7 +13781,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="244" spans="1:13">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>255</v>
       </c>
@@ -13799,7 +13822,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="245" spans="1:13">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>256</v>
       </c>
@@ -13840,7 +13863,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="246" spans="1:13">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>257</v>
       </c>
@@ -13881,7 +13904,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="247" spans="1:13">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>258</v>
       </c>
@@ -13922,7 +13945,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="248" spans="1:13">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>259</v>
       </c>
@@ -13963,7 +13986,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="249" spans="1:13">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>260</v>
       </c>
@@ -14004,7 +14027,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="250" spans="1:13">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>261</v>
       </c>
@@ -14045,7 +14068,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="251" spans="1:13">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>262</v>
       </c>
@@ -14086,7 +14109,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="252" spans="1:13">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>263</v>
       </c>
@@ -14127,7 +14150,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="253" spans="1:13">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>264</v>
       </c>
@@ -14168,7 +14191,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="254" spans="1:13">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>265</v>
       </c>
@@ -14209,7 +14232,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="255" spans="1:13">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>266</v>
       </c>
@@ -14250,7 +14273,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="256" spans="1:13">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>267</v>
       </c>
@@ -14291,7 +14314,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="257" spans="1:13">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>268</v>
       </c>
@@ -14332,7 +14355,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="258" spans="1:13">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>269</v>
       </c>
@@ -14373,7 +14396,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="259" spans="1:13">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>270</v>
       </c>
@@ -14414,7 +14437,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="260" spans="1:13">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>271</v>
       </c>
@@ -14455,7 +14478,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="261" spans="1:13">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>272</v>
       </c>
@@ -14496,7 +14519,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="262" spans="1:13">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>273</v>
       </c>
@@ -14537,7 +14560,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="263" spans="1:13">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>274</v>
       </c>
@@ -14578,7 +14601,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="264" spans="1:13">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>275</v>
       </c>
@@ -14619,7 +14642,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="265" spans="1:13">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>276</v>
       </c>
@@ -14660,7 +14683,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="266" spans="1:13">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>277</v>
       </c>
@@ -14701,7 +14724,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="267" spans="1:13">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>278</v>
       </c>
@@ -14742,7 +14765,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="268" spans="1:13">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>279</v>
       </c>
@@ -14783,7 +14806,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="269" spans="1:13">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>280</v>
       </c>
@@ -14824,7 +14847,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="270" spans="1:13">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>281</v>
       </c>
@@ -14865,7 +14888,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="271" spans="1:13">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>282</v>
       </c>
@@ -14906,7 +14929,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="272" spans="1:13">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>283</v>
       </c>
@@ -14947,7 +14970,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="273" spans="1:13">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>284</v>
       </c>
@@ -14988,7 +15011,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="274" spans="1:13">
+    <row r="274" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>285</v>
       </c>
@@ -15029,7 +15052,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="275" spans="1:13">
+    <row r="275" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>286</v>
       </c>
@@ -15070,7 +15093,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="276" spans="1:13">
+    <row r="276" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>287</v>
       </c>
@@ -15111,7 +15134,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="277" spans="1:13">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>288</v>
       </c>
@@ -15152,7 +15175,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="278" spans="1:13">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>289</v>
       </c>
@@ -15193,7 +15216,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="279" spans="1:13">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>290</v>
       </c>
@@ -15234,7 +15257,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="280" spans="1:13">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>291</v>
       </c>
@@ -15275,7 +15298,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="281" spans="1:13">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>292</v>
       </c>
@@ -15316,7 +15339,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="282" spans="1:13">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>293</v>
       </c>
@@ -15357,7 +15380,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="283" spans="1:13">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>294</v>
       </c>
@@ -15398,7 +15421,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="284" spans="1:13">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>295</v>
       </c>
@@ -15439,7 +15462,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="285" spans="1:13">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>296</v>
       </c>
@@ -15480,7 +15503,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="286" spans="1:13">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>297</v>
       </c>
@@ -15521,7 +15544,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="287" spans="1:13">
+    <row r="287" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>298</v>
       </c>
@@ -15562,7 +15585,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="288" spans="1:13">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>299</v>
       </c>
@@ -15603,7 +15626,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="289" spans="1:13">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>300</v>
       </c>
@@ -15644,7 +15667,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="290" spans="1:13">
+    <row r="290" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>301</v>
       </c>
@@ -15685,7 +15708,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="291" spans="1:13">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>302</v>
       </c>
@@ -15726,7 +15749,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="292" spans="1:13">
+    <row r="292" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>303</v>
       </c>
@@ -15767,7 +15790,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="293" spans="1:13">
+    <row r="293" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>304</v>
       </c>
@@ -15808,7 +15831,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="294" spans="1:13">
+    <row r="294" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>305</v>
       </c>
@@ -15849,7 +15872,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="295" spans="1:13">
+    <row r="295" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>306</v>
       </c>
@@ -15890,7 +15913,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="296" spans="1:13">
+    <row r="296" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>307</v>
       </c>
@@ -15931,7 +15954,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="297" spans="1:13">
+    <row r="297" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>308</v>
       </c>
@@ -15972,7 +15995,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="298" spans="1:13">
+    <row r="298" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>309</v>
       </c>
@@ -16013,7 +16036,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="299" spans="1:13">
+    <row r="299" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>310</v>
       </c>
@@ -16054,7 +16077,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="300" spans="1:13">
+    <row r="300" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>311</v>
       </c>
@@ -16095,7 +16118,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="301" spans="1:13">
+    <row r="301" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>312</v>
       </c>
@@ -16136,7 +16159,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="302" spans="1:13">
+    <row r="302" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>313</v>
       </c>
@@ -16177,7 +16200,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="303" spans="1:13">
+    <row r="303" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>314</v>
       </c>
@@ -16218,7 +16241,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="304" spans="1:13">
+    <row r="304" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>315</v>
       </c>
@@ -16259,7 +16282,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="305" spans="1:13">
+    <row r="305" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>316</v>
       </c>
@@ -16300,7 +16323,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="306" spans="1:13">
+    <row r="306" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>317</v>
       </c>
@@ -16341,7 +16364,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="307" spans="1:13">
+    <row r="307" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>318</v>
       </c>
@@ -16382,7 +16405,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="308" spans="1:13">
+    <row r="308" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>319</v>
       </c>
@@ -16423,7 +16446,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="309" spans="1:13">
+    <row r="309" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>320</v>
       </c>
@@ -16464,7 +16487,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="310" spans="1:13">
+    <row r="310" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>321</v>
       </c>
@@ -16505,7 +16528,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="311" spans="1:13">
+    <row r="311" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>322</v>
       </c>
@@ -16546,7 +16569,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="312" spans="1:13">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>323</v>
       </c>
@@ -16587,7 +16610,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="313" spans="1:13">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>324</v>
       </c>
@@ -16628,7 +16651,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="314" spans="1:13">
+    <row r="314" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>325</v>
       </c>
@@ -16669,7 +16692,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="315" spans="1:13">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>326</v>
       </c>
@@ -16710,7 +16733,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="316" spans="1:13">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>327</v>
       </c>
@@ -16751,7 +16774,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="317" spans="1:13">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>328</v>
       </c>
@@ -16792,7 +16815,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="318" spans="1:13">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>329</v>
       </c>
@@ -16833,7 +16856,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="319" spans="1:13">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>330</v>
       </c>
@@ -16874,7 +16897,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="320" spans="1:13">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>331</v>
       </c>
@@ -16915,7 +16938,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="321" spans="1:13">
+    <row r="321" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>332</v>
       </c>
@@ -16956,7 +16979,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="322" spans="1:13">
+    <row r="322" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>333</v>
       </c>
@@ -16997,7 +17020,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="323" spans="1:13">
+    <row r="323" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>334</v>
       </c>
@@ -17038,7 +17061,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="324" spans="1:13">
+    <row r="324" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>335</v>
       </c>
@@ -17079,7 +17102,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="325" spans="1:13">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>336</v>
       </c>
@@ -17120,7 +17143,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="326" spans="1:13">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>337</v>
       </c>
@@ -17161,7 +17184,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="327" spans="1:13">
+    <row r="327" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>338</v>
       </c>
@@ -17202,7 +17225,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="328" spans="1:13">
+    <row r="328" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>339</v>
       </c>
@@ -17243,7 +17266,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="329" spans="1:13">
+    <row r="329" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>340</v>
       </c>
@@ -17284,7 +17307,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="330" spans="1:13">
+    <row r="330" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>341</v>
       </c>
@@ -17325,7 +17348,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="331" spans="1:13">
+    <row r="331" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>342</v>
       </c>
@@ -17366,7 +17389,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="332" spans="1:13">
+    <row r="332" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>343</v>
       </c>
@@ -17407,7 +17430,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="333" spans="1:13">
+    <row r="333" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>344</v>
       </c>
@@ -17448,7 +17471,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="334" spans="1:13">
+    <row r="334" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>345</v>
       </c>
@@ -17489,7 +17512,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="335" spans="1:13">
+    <row r="335" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>346</v>
       </c>
@@ -17530,7 +17553,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="336" spans="1:13">
+    <row r="336" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>347</v>
       </c>
@@ -17571,7 +17594,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="337" spans="1:13">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>348</v>
       </c>
@@ -17612,7 +17635,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="338" spans="1:13">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>349</v>
       </c>
@@ -17653,7 +17676,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="339" spans="1:13">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>350</v>
       </c>
@@ -17694,7 +17717,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="340" spans="1:13">
+    <row r="340" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>351</v>
       </c>
@@ -17735,7 +17758,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="341" spans="1:13">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>352</v>
       </c>
@@ -17776,7 +17799,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="342" spans="1:13">
+    <row r="342" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>353</v>
       </c>
@@ -17817,7 +17840,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="343" spans="1:13">
+    <row r="343" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>354</v>
       </c>
@@ -17858,7 +17881,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="344" spans="1:13">
+    <row r="344" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>355</v>
       </c>
@@ -17899,7 +17922,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="345" spans="1:13">
+    <row r="345" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>356</v>
       </c>
@@ -17940,7 +17963,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="346" spans="1:13">
+    <row r="346" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>357</v>
       </c>
@@ -17981,7 +18004,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="347" spans="1:13">
+    <row r="347" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>358</v>
       </c>
@@ -18022,7 +18045,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="348" spans="1:13">
+    <row r="348" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>359</v>
       </c>
@@ -18063,7 +18086,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="349" spans="1:13">
+    <row r="349" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>360</v>
       </c>
@@ -18104,7 +18127,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="350" spans="1:13">
+    <row r="350" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>361</v>
       </c>
@@ -18145,7 +18168,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="351" spans="1:13">
+    <row r="351" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>362</v>
       </c>
@@ -18187,6 +18210,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M1"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>

</xml_diff>